<commit_message>
add fillter_data_and_inference.py about read in csv
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-12-19-13-56-None</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.5292857142857142</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ad OnefitallModel and try 1*10 patch for two models
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,36 @@
         <v>0.5292857142857142</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-18-11-18-17-None</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-18-13-54-24-None</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.6785714285714286</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-18-14-14-26-None</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5785714285714286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
finish model 1 2 3 and model 11 12 13
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B10"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,16 @@
         <v>0.6449999999999999</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-20-19-55-06-None</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.7050000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add two bash and add save args
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B11"/>
+  <dimension ref="A2:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,386 @@
         <v>0.7050000000000001</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-14-58-15-Onefitall_11</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.6342857142857141</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-14-58-32-Onefitall_12</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.6364285714285715</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-14-58-48-Onefitall_13</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.6721428571428572</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-14-59-01-LLMFlareNet_1</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.4842857142857143</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-14-59-51-LLMFlareNet_2</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.6464285714285715</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-05-56-Onefitall_11</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.5428571428571429</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-06-00-Onefitall_12</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.5357142857142858</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-06-04-Onefitall_13</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.6285714285714286</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-06-07-LLMFlareNet_1</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.4500000000000001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-06-14-LLMFlareNet_2</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.5571428571428572</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-07-56-Onefitall_11</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.5428571428571429</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-08-00-Onefitall_12</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.5357142857142858</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-08-04-Onefitall_13</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.6285714285714286</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-08-07-LLMFlareNet_1</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.4500000000000001</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-08-15-LLMFlareNet_2</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.5571428571428572</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-09-28-Onefitall_11</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.5428571428571429</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-09-32-Onefitall_12</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.5357142857142858</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-09-36-Onefitall_13</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.6285714285714286</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-09-40-LLMFlareNet_1</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.4500000000000001</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-09-47-LLMFlareNet_2</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.5571428571428572</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-11-24-Onefitall_11</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.5428571428571429</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-11-28-Onefitall_12</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.5357142857142858</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-11-32-Onefitall_13</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.6285714285714286</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-11-36-LLMFlareNet_1</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.4500000000000001</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-11-43-LLMFlareNet_2</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.5571428571428572</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-28-21-Onefitall_11</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.5428571428571429</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-28-25-Onefitall_12</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.5357142857142858</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-28-29-Onefitall_13</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.6285714285714286</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-28-47-Onefitall_11</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.5428571428571429</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-28-51-Onefitall_12</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.5357142857142858</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-28-55-Onefitall_13</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.6285714285714286</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-28-59-LLMFlareNet_1</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.4500000000000001</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-29-06-LLMFlareNet_2</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.5571428571428572</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-29-10-Onefitall_11</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.6071428571428572</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-29-14-Onefitall_12</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.6071428571428572</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-29-18-Onefitall_13</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.6499999999999999</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-29-22-LLMFlareNet_1</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.4571428571428572</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>./model_output/2025-08-22-15-29-29-LLMFlareNet_2</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.5642857142857143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>